<commit_message>
Update 2020Q4 vintage data
</commit_message>
<xml_diff>
--- a/data/vintage_data/data_20201110.xlsx
+++ b/data/vintage_data/data_20201110.xlsx
@@ -53,7 +53,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -2133,7 +2132,7 @@
         <v>0.3205552424323573</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5212973494484274</v>
+        <v>0.521297349448427</v>
       </c>
       <c r="K11" t="n">
         <v>1.586592319685821</v>
@@ -2703,7 +2702,7 @@
         <v>1.933984100271054</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.106410733578875</v>
+        <v>1.106410733578874</v>
       </c>
       <c r="AR14" t="n">
         <v>11.86774686789356</v>
@@ -4832,7 +4831,7 @@
         <v>0.632868546195652</v>
       </c>
       <c r="T28" t="n">
-        <v>0.4435860337334562</v>
+        <v>0.4435860337334561</v>
       </c>
       <c r="U28" t="n">
         <v>0.4259029084872407</v>
@@ -5816,7 +5815,7 @@
         <v>0.07108336656514648</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.2334984651643992</v>
+        <v>0.2334984651643994</v>
       </c>
       <c r="AI34" t="n">
         <v>-0.003003451178451177</v>
@@ -6535,7 +6534,7 @@
         <v>1.61201008939644</v>
       </c>
       <c r="L39" t="n">
-        <v>0.9021102246716857</v>
+        <v>0.9021102246716854</v>
       </c>
       <c r="M39" t="n">
         <v>526.6138468183801</v>
@@ -7872,7 +7871,7 @@
         <v>-0.6152215439932709</v>
       </c>
       <c r="AM47" t="n">
-        <v>2.385855117502017</v>
+        <v>2.385855117502016</v>
       </c>
       <c r="AN47" t="n">
         <v>-4.301546794406078</v>
@@ -8352,7 +8351,7 @@
         <v>0.7096428571428575</v>
       </c>
       <c r="AP50" t="n">
-        <v>0.6715755493938665</v>
+        <v>0.6715755493938667</v>
       </c>
       <c r="AQ50" t="n">
         <v>0.8866227019450581</v>
@@ -11710,10 +11709,10 @@
         <v>0.5137807684662451</v>
       </c>
       <c r="J72" t="n">
-        <v>-0.1951559232039443</v>
+        <v>-0.195155923203944</v>
       </c>
       <c r="K72" t="n">
-        <v>0.8701390470334495</v>
+        <v>0.8701390470334497</v>
       </c>
       <c r="L72" t="n">
         <v>0.3563582785672208</v>
@@ -13850,7 +13849,7 @@
         <v>0.5014685174588395</v>
       </c>
       <c r="AQ85" t="n">
-        <v>0.9973713810507651</v>
+        <v>0.9973713810507652</v>
       </c>
       <c r="AR85" t="n">
         <v>1.49241861685968</v>
@@ -14155,7 +14154,7 @@
         <v>0.9229671322031346</v>
       </c>
       <c r="AN87" t="n">
-        <v>0.9744748058407005</v>
+        <v>0.9744748058407002</v>
       </c>
       <c r="AO87" t="n">
         <v>0.7823260073260079</v>
@@ -15336,7 +15335,7 @@
         <v>1.139607107278304</v>
       </c>
       <c r="O95" t="n">
-        <v>0.5280117495969181</v>
+        <v>0.528011749596918</v>
       </c>
       <c r="P95" t="n">
         <v>0.09650109897146189</v>
@@ -15713,7 +15712,7 @@
         <v>-0.001353451178451177</v>
       </c>
       <c r="AJ97" t="n">
-        <v>-0.05439277572658216</v>
+        <v>-0.05439277572658215</v>
       </c>
       <c r="AK97" t="n">
         <v>-0.3545237186010029</v>
@@ -15852,10 +15851,10 @@
         <v>-2.724194132161244</v>
       </c>
       <c r="AD98" t="n">
-        <v>1.520116133205056</v>
+        <v>-1.026401972744524</v>
       </c>
       <c r="AE98" t="n">
-        <v>0.3764841743469938</v>
+        <v>0.351018993287498</v>
       </c>
       <c r="AF98" t="n">
         <v>0.00776190552552336</v>
@@ -16009,7 +16008,7 @@
         <v>-17.36806875081322</v>
       </c>
       <c r="AD99" t="n">
-        <v>-1.228783079369325</v>
+        <v>1.317735026580265</v>
       </c>
       <c r="AE99" t="n">
         <v>0.3734173101974457</v>
@@ -16159,8 +16158,12 @@
       <c r="AC100" t="n">
         <v>-10.25716212520518</v>
       </c>
-      <c r="AD100" t="inlineStr"/>
-      <c r="AE100" t="inlineStr"/>
+      <c r="AD100" t="n">
+        <v>3.712060737616468</v>
+      </c>
+      <c r="AE100" t="n">
+        <v>0.3996616991546378</v>
+      </c>
       <c r="AF100" t="n">
         <v>-0.08381190777611325</v>
       </c>
@@ -17935,7 +17938,7 @@
         <v>0.3205552424323573</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5212973494484274</v>
+        <v>0.521297349448427</v>
       </c>
       <c r="K11" t="n">
         <v>1.586592319685821</v>
@@ -18505,7 +18508,7 @@
         <v>1.933984100271054</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.106410733578875</v>
+        <v>1.106410733578874</v>
       </c>
       <c r="AR14" t="n">
         <v>11.86774686789356</v>
@@ -20634,7 +20637,7 @@
         <v>0.632868546195652</v>
       </c>
       <c r="T28" t="n">
-        <v>0.4435860337334562</v>
+        <v>0.4435860337334561</v>
       </c>
       <c r="U28" t="n">
         <v>0.4259029084872407</v>
@@ -21618,7 +21621,7 @@
         <v>0.07108336656514648</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.2334984651643992</v>
+        <v>0.2334984651643994</v>
       </c>
       <c r="AI34" t="n">
         <v>-0.003003451178451177</v>
@@ -22337,7 +22340,7 @@
         <v>1.61201008939644</v>
       </c>
       <c r="L39" t="n">
-        <v>0.9021102246716857</v>
+        <v>0.9021102246716854</v>
       </c>
       <c r="M39" t="n">
         <v>526.6138468183801</v>
@@ -23674,7 +23677,7 @@
         <v>-0.6152215439932709</v>
       </c>
       <c r="AM47" t="n">
-        <v>2.385855117502017</v>
+        <v>2.385855117502016</v>
       </c>
       <c r="AN47" t="n">
         <v>-4.301546794406078</v>
@@ -24154,7 +24157,7 @@
         <v>0.7096428571428575</v>
       </c>
       <c r="AP50" t="n">
-        <v>0.6715755493938665</v>
+        <v>0.6715755493938667</v>
       </c>
       <c r="AQ50" t="n">
         <v>0.8866227019450581</v>
@@ -27512,10 +27515,10 @@
         <v>0.5137807684662451</v>
       </c>
       <c r="J72" t="n">
-        <v>-0.1951559232039443</v>
+        <v>-0.195155923203944</v>
       </c>
       <c r="K72" t="n">
-        <v>0.8701390470334495</v>
+        <v>0.8701390470334497</v>
       </c>
       <c r="L72" t="n">
         <v>0.3563582785672208</v>
@@ -29652,7 +29655,7 @@
         <v>0.5014685174588395</v>
       </c>
       <c r="AQ85" t="n">
-        <v>0.9973713810507651</v>
+        <v>0.9973713810507652</v>
       </c>
       <c r="AR85" t="n">
         <v>1.49241861685968</v>
@@ -29957,7 +29960,7 @@
         <v>0.9229671322031346</v>
       </c>
       <c r="AN87" t="n">
-        <v>0.9744748058407005</v>
+        <v>0.9744748058407002</v>
       </c>
       <c r="AO87" t="n">
         <v>0.7823260073260079</v>
@@ -31138,7 +31141,7 @@
         <v>1.139607107278304</v>
       </c>
       <c r="O95" t="n">
-        <v>0.5280117495969181</v>
+        <v>0.528011749596918</v>
       </c>
       <c r="P95" t="n">
         <v>0.09650109897146189</v>
@@ -31515,7 +31518,7 @@
         <v>-0.001353451178451177</v>
       </c>
       <c r="AJ97" t="n">
-        <v>-0.05439277572658216</v>
+        <v>-0.05439277572658215</v>
       </c>
       <c r="AK97" t="n">
         <v>-0.3545237186010029</v>
@@ -31654,10 +31657,10 @@
         <v>-2.724194132161244</v>
       </c>
       <c r="AD98" t="n">
-        <v>1.520116133205056</v>
+        <v>-1.026401972744524</v>
       </c>
       <c r="AE98" t="n">
-        <v>0.3764841743469938</v>
+        <v>0.351018993287498</v>
       </c>
       <c r="AF98" t="n">
         <v>0.00776190552552336</v>
@@ -31811,7 +31814,7 @@
         <v>-17.36806875081322</v>
       </c>
       <c r="AD99" t="n">
-        <v>-1.228783079369325</v>
+        <v>1.317735026580265</v>
       </c>
       <c r="AE99" t="n">
         <v>0.3734173101974457</v>
@@ -31961,8 +31964,12 @@
       <c r="AC100" t="n">
         <v>-10.25716212520518</v>
       </c>
-      <c r="AD100" t="inlineStr"/>
-      <c r="AE100" t="inlineStr"/>
+      <c r="AD100" t="n">
+        <v>3.712060737616468</v>
+      </c>
+      <c r="AE100" t="n">
+        <v>0.3996616991546378</v>
+      </c>
       <c r="AF100" t="n">
         <v>-0.08381190777611325</v>
       </c>
@@ -33808,7 +33815,7 @@
         <v>0.3205552424323573</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5212973494484274</v>
+        <v>0.521297349448427</v>
       </c>
       <c r="K11" t="n">
         <v>1.586592319685821</v>
@@ -34378,7 +34385,7 @@
         <v>1.933984100271054</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.106410733578875</v>
+        <v>1.106410733578874</v>
       </c>
       <c r="AR14" t="n">
         <v>11.86774686789356</v>
@@ -36507,7 +36514,7 @@
         <v>0.632868546195652</v>
       </c>
       <c r="T28" t="n">
-        <v>0.4435860337334562</v>
+        <v>0.4435860337334561</v>
       </c>
       <c r="U28" t="n">
         <v>0.4259029084872407</v>
@@ -37491,7 +37498,7 @@
         <v>0.07108336656514648</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.2334984651643992</v>
+        <v>0.2334984651643994</v>
       </c>
       <c r="AI34" t="n">
         <v>-0.003003451178451177</v>
@@ -38210,7 +38217,7 @@
         <v>1.61201008939644</v>
       </c>
       <c r="L39" t="n">
-        <v>0.9021102246716857</v>
+        <v>0.9021102246716854</v>
       </c>
       <c r="M39" t="n">
         <v>526.6138468183801</v>
@@ -39547,7 +39554,7 @@
         <v>-0.6152215439932709</v>
       </c>
       <c r="AM47" t="n">
-        <v>2.385855117502017</v>
+        <v>2.385855117502016</v>
       </c>
       <c r="AN47" t="n">
         <v>-4.301546794406078</v>
@@ -40027,7 +40034,7 @@
         <v>0.7096428571428575</v>
       </c>
       <c r="AP50" t="n">
-        <v>0.6715755493938665</v>
+        <v>0.6715755493938667</v>
       </c>
       <c r="AQ50" t="n">
         <v>0.8866227019450581</v>
@@ -43385,10 +43392,10 @@
         <v>0.5137807684662451</v>
       </c>
       <c r="J72" t="n">
-        <v>-0.1951559232039443</v>
+        <v>-0.195155923203944</v>
       </c>
       <c r="K72" t="n">
-        <v>0.8701390470334495</v>
+        <v>0.8701390470334497</v>
       </c>
       <c r="L72" t="n">
         <v>0.3563582785672208</v>
@@ -45525,7 +45532,7 @@
         <v>0.5014685174588395</v>
       </c>
       <c r="AQ85" t="n">
-        <v>0.9973713810507651</v>
+        <v>0.9973713810507652</v>
       </c>
       <c r="AR85" t="n">
         <v>1.49241861685968</v>
@@ -45830,7 +45837,7 @@
         <v>0.9229671322031346</v>
       </c>
       <c r="AN87" t="n">
-        <v>0.9744748058407005</v>
+        <v>0.9744748058407002</v>
       </c>
       <c r="AO87" t="n">
         <v>0.7823260073260079</v>
@@ -47011,7 +47018,7 @@
         <v>1.139607107278304</v>
       </c>
       <c r="O95" t="n">
-        <v>0.5280117495969181</v>
+        <v>0.528011749596918</v>
       </c>
       <c r="P95" t="n">
         <v>0.09650109897146189</v>
@@ -47388,7 +47395,7 @@
         <v>-0.001353451178451177</v>
       </c>
       <c r="AJ97" t="n">
-        <v>-0.05439277572658216</v>
+        <v>-0.05439277572658215</v>
       </c>
       <c r="AK97" t="n">
         <v>-0.3545237186010029</v>
@@ -47527,10 +47534,10 @@
         <v>-2.724194132161244</v>
       </c>
       <c r="AD98" t="n">
-        <v>1.520116133205056</v>
+        <v>-1.026401972744524</v>
       </c>
       <c r="AE98" t="n">
-        <v>0.3764841743469938</v>
+        <v>0.351018993287498</v>
       </c>
       <c r="AF98" t="n">
         <v>0.00776190552552336</v>
@@ -47684,7 +47691,7 @@
         <v>-17.36806875081322</v>
       </c>
       <c r="AD99" t="n">
-        <v>-1.228783079369325</v>
+        <v>1.317735026580265</v>
       </c>
       <c r="AE99" t="n">
         <v>0.3734173101974457</v>
@@ -47834,8 +47841,12 @@
       <c r="AC100" t="n">
         <v>-10.25716212520518</v>
       </c>
-      <c r="AD100" t="inlineStr"/>
-      <c r="AE100" t="inlineStr"/>
+      <c r="AD100" t="n">
+        <v>3.712060737616468</v>
+      </c>
+      <c r="AE100" t="n">
+        <v>0.3996616991546378</v>
+      </c>
       <c r="AF100" t="n">
         <v>-0.08381190777611325</v>
       </c>
@@ -49695,7 +49706,7 @@
         <v>0.3205552424323573</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5212973494484274</v>
+        <v>0.521297349448427</v>
       </c>
       <c r="K11" t="n">
         <v>1.586592319685821</v>
@@ -50265,7 +50276,7 @@
         <v>1.933984100271054</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.106410733578875</v>
+        <v>1.106410733578874</v>
       </c>
       <c r="AR14" t="n">
         <v>11.86774686789356</v>
@@ -52394,7 +52405,7 @@
         <v>0.632868546195652</v>
       </c>
       <c r="T28" t="n">
-        <v>0.4435860337334562</v>
+        <v>0.4435860337334561</v>
       </c>
       <c r="U28" t="n">
         <v>0.4259029084872407</v>
@@ -53378,7 +53389,7 @@
         <v>0.07108336656514648</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.2334984651643992</v>
+        <v>0.2334984651643994</v>
       </c>
       <c r="AI34" t="n">
         <v>-0.003003451178451177</v>
@@ -54097,7 +54108,7 @@
         <v>1.61201008939644</v>
       </c>
       <c r="L39" t="n">
-        <v>0.9021102246716857</v>
+        <v>0.9021102246716854</v>
       </c>
       <c r="M39" t="n">
         <v>526.6138468183801</v>
@@ -55434,7 +55445,7 @@
         <v>-0.6152215439932709</v>
       </c>
       <c r="AM47" t="n">
-        <v>2.385855117502017</v>
+        <v>2.385855117502016</v>
       </c>
       <c r="AN47" t="n">
         <v>-4.301546794406078</v>
@@ -55914,7 +55925,7 @@
         <v>0.7096428571428575</v>
       </c>
       <c r="AP50" t="n">
-        <v>0.6715755493938665</v>
+        <v>0.6715755493938667</v>
       </c>
       <c r="AQ50" t="n">
         <v>0.8866227019450581</v>
@@ -59272,10 +59283,10 @@
         <v>0.5137807684662451</v>
       </c>
       <c r="J72" t="n">
-        <v>-0.1951559232039443</v>
+        <v>-0.195155923203944</v>
       </c>
       <c r="K72" t="n">
-        <v>0.8701390470334495</v>
+        <v>0.8701390470334497</v>
       </c>
       <c r="L72" t="n">
         <v>0.3563582785672208</v>
@@ -61412,7 +61423,7 @@
         <v>0.5014685174588395</v>
       </c>
       <c r="AQ85" t="n">
-        <v>0.9973713810507651</v>
+        <v>0.9973713810507652</v>
       </c>
       <c r="AR85" t="n">
         <v>1.49241861685968</v>
@@ -61717,7 +61728,7 @@
         <v>0.9229671322031346</v>
       </c>
       <c r="AN87" t="n">
-        <v>0.9744748058407005</v>
+        <v>0.9744748058407002</v>
       </c>
       <c r="AO87" t="n">
         <v>0.7823260073260079</v>
@@ -62898,7 +62909,7 @@
         <v>1.139607107278304</v>
       </c>
       <c r="O95" t="n">
-        <v>0.5280117495969181</v>
+        <v>0.528011749596918</v>
       </c>
       <c r="P95" t="n">
         <v>0.09650109897146189</v>
@@ -63275,7 +63286,7 @@
         <v>-0.001353451178451177</v>
       </c>
       <c r="AJ97" t="n">
-        <v>-0.05439277572658216</v>
+        <v>-0.05439277572658215</v>
       </c>
       <c r="AK97" t="n">
         <v>-0.3545237186010029</v>
@@ -63414,10 +63425,10 @@
         <v>-2.724194132161244</v>
       </c>
       <c r="AD98" t="n">
-        <v>1.520116133205056</v>
+        <v>-1.026401972744524</v>
       </c>
       <c r="AE98" t="n">
-        <v>0.3764841743469938</v>
+        <v>0.351018993287498</v>
       </c>
       <c r="AF98" t="n">
         <v>0.00776190552552336</v>
@@ -63571,7 +63582,7 @@
         <v>-17.36806875081322</v>
       </c>
       <c r="AD99" t="n">
-        <v>-1.228783079369325</v>
+        <v>1.317735026580265</v>
       </c>
       <c r="AE99" t="n">
         <v>0.3734173101974457</v>
@@ -63721,8 +63732,12 @@
       <c r="AC100" t="n">
         <v>-10.25716212520518</v>
       </c>
-      <c r="AD100" t="inlineStr"/>
-      <c r="AE100" t="inlineStr"/>
+      <c r="AD100" t="n">
+        <v>3.712060737616468</v>
+      </c>
+      <c r="AE100" t="n">
+        <v>0.3996616991546378</v>
+      </c>
       <c r="AF100" t="n">
         <v>-0.08381190777611325</v>
       </c>

</xml_diff>